<commit_message>
planning update and camera problem correction
</commit_message>
<xml_diff>
--- a/docs/Kinetoscope_TB_planning.xlsx
+++ b/docs/Kinetoscope_TB_planning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kilian.brandtdi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kilian.brandtdi\Documents\Visual Studio 2013\xvision\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -653,7 +653,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -696,19 +696,38 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -720,34 +739,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1055,7 +1057,7 @@
   <dimension ref="A1:AM45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1064,10 +1066,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
+      <c r="B1" s="43"/>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1181,13 +1183,13 @@
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="52">
+      <c r="B2" s="47">
         <v>1</v>
       </c>
-      <c r="C2" s="55" t="s">
+      <c r="C2" s="46" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="4"/>
@@ -1228,11 +1230,11 @@
       <c r="AM2" s="6"/>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A3" s="48"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="27"/>
+      <c r="A3" s="55"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="61"/>
       <c r="F3" s="22"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -1269,11 +1271,11 @@
       <c r="AM3" s="9"/>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A4" s="48"/>
-      <c r="B4" s="43">
+      <c r="A4" s="55"/>
+      <c r="B4" s="48">
         <v>2</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="44" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="10"/>
@@ -1314,11 +1316,11 @@
       <c r="AM4" s="9"/>
     </row>
     <row r="5" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="49"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="51"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="45"/>
       <c r="D5" s="12"/>
-      <c r="E5" s="29"/>
+      <c r="E5" s="60"/>
       <c r="F5" s="23"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
@@ -1355,13 +1357,13 @@
       <c r="AM5" s="14"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="52">
+      <c r="B6" s="47">
         <v>1</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="46" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="15"/>
@@ -1402,11 +1404,11 @@
       <c r="AM6" s="6"/>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A7" s="48"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="50"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="27"/>
+      <c r="E7" s="61"/>
       <c r="F7" s="22"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
@@ -1443,11 +1445,11 @@
       <c r="AM7" s="9"/>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A8" s="48"/>
-      <c r="B8" s="43">
+      <c r="A8" s="55"/>
+      <c r="B8" s="48">
         <v>2</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="44" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="7"/>
@@ -1488,11 +1490,11 @@
       <c r="AM8" s="9"/>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A9" s="48"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="50"/>
+      <c r="A9" s="55"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="27"/>
+      <c r="E9" s="61"/>
       <c r="F9" s="22"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -1529,11 +1531,11 @@
       <c r="AM9" s="9"/>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A10" s="48"/>
-      <c r="B10" s="43">
+      <c r="A10" s="55"/>
+      <c r="B10" s="48">
         <v>3</v>
       </c>
-      <c r="C10" s="50" t="s">
+      <c r="C10" s="44" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="7"/>
@@ -1574,11 +1576,11 @@
       <c r="AM10" s="9"/>
     </row>
     <row r="11" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="49"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="51"/>
+      <c r="A11" s="56"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="45"/>
       <c r="D11" s="12"/>
-      <c r="E11" s="29"/>
+      <c r="E11" s="60"/>
       <c r="F11" s="23"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
@@ -1615,13 +1617,13 @@
       <c r="AM11" s="14"/>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A12" s="56" t="s">
+      <c r="A12" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="45">
+      <c r="B12" s="51">
         <v>1</v>
       </c>
-      <c r="C12" s="53" t="s">
+      <c r="C12" s="49" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="15"/>
@@ -1662,9 +1664,9 @@
       <c r="AM12" s="6"/>
     </row>
     <row r="13" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="57"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="54"/>
+      <c r="A13" s="58"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="12"/>
       <c r="E13" s="29"/>
       <c r="F13" s="23"/>
@@ -1703,13 +1705,13 @@
       <c r="AM13" s="14"/>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A14" s="56" t="s">
+      <c r="A14" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="45">
+      <c r="B14" s="51">
         <v>1</v>
       </c>
-      <c r="C14" s="53" t="s">
+      <c r="C14" s="49" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="15"/>
@@ -1750,9 +1752,9 @@
       <c r="AM14" s="6"/>
     </row>
     <row r="15" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="57"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="54"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="12"/>
       <c r="E15" s="29"/>
       <c r="F15" s="23"/>
@@ -1791,13 +1793,13 @@
       <c r="AM15" s="14"/>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="52">
+      <c r="B16" s="47">
         <v>1</v>
       </c>
-      <c r="C16" s="55" t="s">
+      <c r="C16" s="46" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="15"/>
@@ -1838,9 +1840,9 @@
       <c r="AM16" s="6"/>
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A17" s="48"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="50"/>
+      <c r="A17" s="55"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="44"/>
       <c r="D17" s="7"/>
       <c r="E17" s="27"/>
       <c r="F17" s="22"/>
@@ -1879,11 +1881,11 @@
       <c r="AM17" s="9"/>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A18" s="48"/>
-      <c r="B18" s="43">
+      <c r="A18" s="55"/>
+      <c r="B18" s="48">
         <v>2</v>
       </c>
-      <c r="C18" s="50" t="s">
+      <c r="C18" s="44" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="7"/>
@@ -1924,9 +1926,9 @@
       <c r="AM18" s="9"/>
     </row>
     <row r="19" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="49"/>
-      <c r="B19" s="44"/>
-      <c r="C19" s="51"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="45"/>
       <c r="D19" s="12"/>
       <c r="E19" s="29"/>
       <c r="F19" s="23"/>
@@ -1965,13 +1967,13 @@
       <c r="AM19" s="14"/>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="52">
+      <c r="B20" s="47">
         <v>1</v>
       </c>
-      <c r="C20" s="55" t="s">
+      <c r="C20" s="46" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="15"/>
@@ -2012,9 +2014,9 @@
       <c r="AM20" s="6"/>
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A21" s="48"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="50"/>
+      <c r="A21" s="55"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="44"/>
       <c r="D21" s="7"/>
       <c r="E21" s="27"/>
       <c r="F21" s="22"/>
@@ -2053,11 +2055,11 @@
       <c r="AM21" s="9"/>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A22" s="48"/>
-      <c r="B22" s="43">
+      <c r="A22" s="55"/>
+      <c r="B22" s="48">
         <v>2</v>
       </c>
-      <c r="C22" s="50" t="s">
+      <c r="C22" s="44" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="7"/>
@@ -2098,9 +2100,9 @@
       <c r="AM22" s="9"/>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A23" s="48"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="50"/>
+      <c r="A23" s="55"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="44"/>
       <c r="D23" s="7"/>
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
@@ -2139,11 +2141,11 @@
       <c r="AM23" s="9"/>
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A24" s="48"/>
-      <c r="B24" s="43">
+      <c r="A24" s="55"/>
+      <c r="B24" s="48">
         <v>3</v>
       </c>
-      <c r="C24" s="50" t="s">
+      <c r="C24" s="44" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="7"/>
@@ -2184,9 +2186,9 @@
       <c r="AM24" s="9"/>
     </row>
     <row r="25" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="49"/>
-      <c r="B25" s="44"/>
-      <c r="C25" s="51"/>
+      <c r="A25" s="56"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="45"/>
       <c r="D25" s="12"/>
       <c r="E25" s="29"/>
       <c r="F25" s="23"/>
@@ -2225,13 +2227,13 @@
       <c r="AM25" s="14"/>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A26" s="56" t="s">
+      <c r="A26" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="45">
+      <c r="B26" s="51">
         <v>1</v>
       </c>
-      <c r="C26" s="53" t="s">
+      <c r="C26" s="49" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="15"/>
@@ -2272,9 +2274,9 @@
       <c r="AM26" s="20"/>
     </row>
     <row r="27" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="57"/>
-      <c r="B27" s="46"/>
-      <c r="C27" s="54"/>
+      <c r="A27" s="58"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="50"/>
       <c r="D27" s="12"/>
       <c r="E27" s="29"/>
       <c r="F27" s="23"/>
@@ -2313,13 +2315,13 @@
       <c r="AM27" s="14"/>
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A28" s="47" t="s">
+      <c r="A28" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="52">
+      <c r="B28" s="47">
         <v>1</v>
       </c>
-      <c r="C28" s="55" t="s">
+      <c r="C28" s="46" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="17"/>
@@ -2360,9 +2362,9 @@
       <c r="AM28" s="6"/>
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A29" s="48"/>
-      <c r="B29" s="43"/>
-      <c r="C29" s="50"/>
+      <c r="A29" s="55"/>
+      <c r="B29" s="48"/>
+      <c r="C29" s="44"/>
       <c r="D29" s="7"/>
       <c r="E29" s="27"/>
       <c r="F29" s="22"/>
@@ -2401,11 +2403,11 @@
       <c r="AM29" s="9"/>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A30" s="48"/>
-      <c r="B30" s="43">
+      <c r="A30" s="55"/>
+      <c r="B30" s="48">
         <v>2</v>
       </c>
-      <c r="C30" s="50" t="s">
+      <c r="C30" s="44" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="7"/>
@@ -2446,9 +2448,9 @@
       <c r="AM30" s="19"/>
     </row>
     <row r="31" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="49"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="51"/>
+      <c r="A31" s="56"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="45"/>
       <c r="D31" s="12"/>
       <c r="E31" s="29"/>
       <c r="F31" s="23"/>
@@ -2534,54 +2536,54 @@
         <v>27</v>
       </c>
       <c r="G36" s="34"/>
-      <c r="J36" s="42" t="s">
+      <c r="J36" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="K36" s="42"/>
-      <c r="L36" s="42"/>
-      <c r="M36" s="42"/>
-      <c r="N36" s="42" t="s">
+      <c r="K36" s="59"/>
+      <c r="L36" s="59"/>
+      <c r="M36" s="59"/>
+      <c r="N36" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="O36" s="42"/>
-      <c r="P36" s="42"/>
-      <c r="Q36" s="42"/>
-      <c r="R36" s="42"/>
-      <c r="V36" s="42" t="s">
+      <c r="O36" s="59"/>
+      <c r="P36" s="59"/>
+      <c r="Q36" s="59"/>
+      <c r="R36" s="59"/>
+      <c r="V36" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="W36" s="42"/>
-      <c r="X36" s="42"/>
-      <c r="Y36" s="42"/>
-      <c r="Z36" s="42"/>
-      <c r="AC36" s="42" t="s">
+      <c r="W36" s="59"/>
+      <c r="X36" s="59"/>
+      <c r="Y36" s="59"/>
+      <c r="Z36" s="59"/>
+      <c r="AC36" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="AD36" s="42"/>
-      <c r="AE36" s="42"/>
-      <c r="AF36" s="42"/>
-      <c r="AG36" s="42"/>
+      <c r="AD36" s="59"/>
+      <c r="AE36" s="59"/>
+      <c r="AF36" s="59"/>
+      <c r="AG36" s="59"/>
     </row>
     <row r="37" spans="5:33" x14ac:dyDescent="0.3">
-      <c r="J37" s="42"/>
-      <c r="K37" s="42"/>
-      <c r="L37" s="42"/>
-      <c r="M37" s="42"/>
-      <c r="N37" s="42"/>
-      <c r="O37" s="42"/>
-      <c r="P37" s="42"/>
-      <c r="Q37" s="42"/>
-      <c r="R37" s="42"/>
-      <c r="V37" s="42"/>
-      <c r="W37" s="42"/>
-      <c r="X37" s="42"/>
-      <c r="Y37" s="42"/>
-      <c r="Z37" s="42"/>
-      <c r="AC37" s="42"/>
-      <c r="AD37" s="42"/>
-      <c r="AE37" s="42"/>
-      <c r="AF37" s="42"/>
-      <c r="AG37" s="42"/>
+      <c r="J37" s="59"/>
+      <c r="K37" s="59"/>
+      <c r="L37" s="59"/>
+      <c r="M37" s="59"/>
+      <c r="N37" s="59"/>
+      <c r="O37" s="59"/>
+      <c r="P37" s="59"/>
+      <c r="Q37" s="59"/>
+      <c r="R37" s="59"/>
+      <c r="V37" s="59"/>
+      <c r="W37" s="59"/>
+      <c r="X37" s="59"/>
+      <c r="Y37" s="59"/>
+      <c r="Z37" s="59"/>
+      <c r="AC37" s="59"/>
+      <c r="AD37" s="59"/>
+      <c r="AE37" s="59"/>
+      <c r="AF37" s="59"/>
+      <c r="AG37" s="59"/>
     </row>
     <row r="42" spans="5:33" x14ac:dyDescent="0.3">
       <c r="F42" s="2"/>
@@ -2609,6 +2611,36 @@
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="AC36:AF37"/>
+    <mergeCell ref="AG36:AG37"/>
+    <mergeCell ref="J36:M37"/>
+    <mergeCell ref="N36:Q37"/>
+    <mergeCell ref="R36:R37"/>
+    <mergeCell ref="V36:Y37"/>
+    <mergeCell ref="Z36:Z37"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="C20:C21"/>
@@ -2625,36 +2657,6 @@
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="AC36:AF37"/>
-    <mergeCell ref="AG36:AG37"/>
-    <mergeCell ref="J36:M37"/>
-    <mergeCell ref="N36:Q37"/>
-    <mergeCell ref="R36:R37"/>
-    <mergeCell ref="V36:Y37"/>
-    <mergeCell ref="Z36:Z37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
error message when config loading fail and config loading now ok but still absolute path
</commit_message>
<xml_diff>
--- a/docs/Kinetoscope_TB_planning.xlsx
+++ b/docs/Kinetoscope_TB_planning.xlsx
@@ -697,37 +697,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -739,17 +723,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1056,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1066,10 +1066,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="61"/>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1183,13 +1183,13 @@
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="47">
+      <c r="B2" s="55">
         <v>1</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="58" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="4"/>
@@ -1230,11 +1230,11 @@
       <c r="AM2" s="6"/>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A3" s="55"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="44"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="53"/>
       <c r="D3" s="42"/>
-      <c r="E3" s="61"/>
+      <c r="E3" s="44"/>
       <c r="F3" s="22"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -1271,11 +1271,11 @@
       <c r="AM3" s="9"/>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A4" s="55"/>
-      <c r="B4" s="48">
+      <c r="A4" s="51"/>
+      <c r="B4" s="46">
         <v>2</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="53" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="10"/>
@@ -1316,11 +1316,11 @@
       <c r="AM4" s="9"/>
     </row>
     <row r="5" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="56"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="45"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="54"/>
       <c r="D5" s="12"/>
-      <c r="E5" s="60"/>
+      <c r="E5" s="43"/>
       <c r="F5" s="23"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
@@ -1357,13 +1357,13 @@
       <c r="AM5" s="14"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="47">
+      <c r="B6" s="55">
         <v>1</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="58" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="15"/>
@@ -1404,11 +1404,11 @@
       <c r="AM6" s="6"/>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A7" s="55"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="44"/>
+      <c r="A7" s="51"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="53"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="61"/>
+      <c r="E7" s="44"/>
       <c r="F7" s="22"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
@@ -1445,11 +1445,11 @@
       <c r="AM7" s="9"/>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A8" s="55"/>
-      <c r="B8" s="48">
+      <c r="A8" s="51"/>
+      <c r="B8" s="46">
         <v>2</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="53" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="7"/>
@@ -1490,11 +1490,11 @@
       <c r="AM8" s="9"/>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A9" s="55"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="44"/>
+      <c r="A9" s="51"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="53"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="61"/>
+      <c r="E9" s="44"/>
       <c r="F9" s="22"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -1531,11 +1531,11 @@
       <c r="AM9" s="9"/>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A10" s="55"/>
-      <c r="B10" s="48">
+      <c r="A10" s="51"/>
+      <c r="B10" s="46">
         <v>3</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="53" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="7"/>
@@ -1576,11 +1576,11 @@
       <c r="AM10" s="9"/>
     </row>
     <row r="11" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="56"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="45"/>
+      <c r="A11" s="52"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="54"/>
       <c r="D11" s="12"/>
-      <c r="E11" s="60"/>
+      <c r="E11" s="43"/>
       <c r="F11" s="23"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
@@ -1617,13 +1617,13 @@
       <c r="AM11" s="14"/>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="51">
+      <c r="B12" s="48">
         <v>1</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="56" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="15"/>
@@ -1664,9 +1664,9 @@
       <c r="AM12" s="6"/>
     </row>
     <row r="13" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="58"/>
-      <c r="B13" s="52"/>
-      <c r="C13" s="50"/>
+      <c r="A13" s="60"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="57"/>
       <c r="D13" s="12"/>
       <c r="E13" s="29"/>
       <c r="F13" s="23"/>
@@ -1705,13 +1705,13 @@
       <c r="AM13" s="14"/>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="51">
+      <c r="B14" s="48">
         <v>1</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="56" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="15"/>
@@ -1752,9 +1752,9 @@
       <c r="AM14" s="6"/>
     </row>
     <row r="15" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="58"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="50"/>
+      <c r="A15" s="60"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="57"/>
       <c r="D15" s="12"/>
       <c r="E15" s="29"/>
       <c r="F15" s="23"/>
@@ -1793,13 +1793,13 @@
       <c r="AM15" s="14"/>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="47">
+      <c r="B16" s="55">
         <v>1</v>
       </c>
-      <c r="C16" s="46" t="s">
+      <c r="C16" s="58" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="15"/>
@@ -1840,9 +1840,9 @@
       <c r="AM16" s="6"/>
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A17" s="55"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="44"/>
+      <c r="A17" s="51"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="53"/>
       <c r="D17" s="7"/>
       <c r="E17" s="27"/>
       <c r="F17" s="22"/>
@@ -1881,11 +1881,11 @@
       <c r="AM17" s="9"/>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A18" s="55"/>
-      <c r="B18" s="48">
+      <c r="A18" s="51"/>
+      <c r="B18" s="46">
         <v>2</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="53" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="7"/>
@@ -1926,9 +1926,9 @@
       <c r="AM18" s="9"/>
     </row>
     <row r="19" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="56"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="45"/>
+      <c r="A19" s="52"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="54"/>
       <c r="D19" s="12"/>
       <c r="E19" s="29"/>
       <c r="F19" s="23"/>
@@ -1967,13 +1967,13 @@
       <c r="AM19" s="14"/>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A20" s="54" t="s">
+      <c r="A20" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="47">
+      <c r="B20" s="55">
         <v>1</v>
       </c>
-      <c r="C20" s="46" t="s">
+      <c r="C20" s="58" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="15"/>
@@ -2014,9 +2014,9 @@
       <c r="AM20" s="6"/>
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A21" s="55"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="44"/>
+      <c r="A21" s="51"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="53"/>
       <c r="D21" s="7"/>
       <c r="E21" s="27"/>
       <c r="F21" s="22"/>
@@ -2055,11 +2055,11 @@
       <c r="AM21" s="9"/>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A22" s="55"/>
-      <c r="B22" s="48">
+      <c r="A22" s="51"/>
+      <c r="B22" s="46">
         <v>2</v>
       </c>
-      <c r="C22" s="44" t="s">
+      <c r="C22" s="53" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="7"/>
@@ -2100,9 +2100,9 @@
       <c r="AM22" s="9"/>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A23" s="55"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="44"/>
+      <c r="A23" s="51"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="53"/>
       <c r="D23" s="7"/>
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
@@ -2141,11 +2141,11 @@
       <c r="AM23" s="9"/>
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A24" s="55"/>
-      <c r="B24" s="48">
+      <c r="A24" s="51"/>
+      <c r="B24" s="46">
         <v>3</v>
       </c>
-      <c r="C24" s="44" t="s">
+      <c r="C24" s="53" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="7"/>
@@ -2186,9 +2186,9 @@
       <c r="AM24" s="9"/>
     </row>
     <row r="25" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="56"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="45"/>
+      <c r="A25" s="52"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="54"/>
       <c r="D25" s="12"/>
       <c r="E25" s="29"/>
       <c r="F25" s="23"/>
@@ -2227,13 +2227,13 @@
       <c r="AM25" s="14"/>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A26" s="57" t="s">
+      <c r="A26" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="51">
+      <c r="B26" s="48">
         <v>1</v>
       </c>
-      <c r="C26" s="49" t="s">
+      <c r="C26" s="56" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="15"/>
@@ -2274,9 +2274,9 @@
       <c r="AM26" s="20"/>
     </row>
     <row r="27" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="58"/>
-      <c r="B27" s="52"/>
-      <c r="C27" s="50"/>
+      <c r="A27" s="60"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="57"/>
       <c r="D27" s="12"/>
       <c r="E27" s="29"/>
       <c r="F27" s="23"/>
@@ -2315,13 +2315,13 @@
       <c r="AM27" s="14"/>
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="47">
+      <c r="B28" s="55">
         <v>1</v>
       </c>
-      <c r="C28" s="46" t="s">
+      <c r="C28" s="58" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="17"/>
@@ -2362,9 +2362,9 @@
       <c r="AM28" s="6"/>
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A29" s="55"/>
-      <c r="B29" s="48"/>
-      <c r="C29" s="44"/>
+      <c r="A29" s="51"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="53"/>
       <c r="D29" s="7"/>
       <c r="E29" s="27"/>
       <c r="F29" s="22"/>
@@ -2403,11 +2403,11 @@
       <c r="AM29" s="9"/>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A30" s="55"/>
-      <c r="B30" s="48">
+      <c r="A30" s="51"/>
+      <c r="B30" s="46">
         <v>2</v>
       </c>
-      <c r="C30" s="44" t="s">
+      <c r="C30" s="53" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="7"/>
@@ -2448,9 +2448,9 @@
       <c r="AM30" s="19"/>
     </row>
     <row r="31" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="56"/>
-      <c r="B31" s="53"/>
-      <c r="C31" s="45"/>
+      <c r="A31" s="52"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="54"/>
       <c r="D31" s="12"/>
       <c r="E31" s="29"/>
       <c r="F31" s="23"/>
@@ -2536,54 +2536,54 @@
         <v>27</v>
       </c>
       <c r="G36" s="34"/>
-      <c r="J36" s="59" t="s">
+      <c r="J36" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="K36" s="59"/>
-      <c r="L36" s="59"/>
-      <c r="M36" s="59"/>
-      <c r="N36" s="59" t="s">
+      <c r="K36" s="45"/>
+      <c r="L36" s="45"/>
+      <c r="M36" s="45"/>
+      <c r="N36" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="O36" s="59"/>
-      <c r="P36" s="59"/>
-      <c r="Q36" s="59"/>
-      <c r="R36" s="59"/>
-      <c r="V36" s="59" t="s">
+      <c r="O36" s="45"/>
+      <c r="P36" s="45"/>
+      <c r="Q36" s="45"/>
+      <c r="R36" s="45"/>
+      <c r="V36" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="W36" s="59"/>
-      <c r="X36" s="59"/>
-      <c r="Y36" s="59"/>
-      <c r="Z36" s="59"/>
-      <c r="AC36" s="59" t="s">
+      <c r="W36" s="45"/>
+      <c r="X36" s="45"/>
+      <c r="Y36" s="45"/>
+      <c r="Z36" s="45"/>
+      <c r="AC36" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="AD36" s="59"/>
-      <c r="AE36" s="59"/>
-      <c r="AF36" s="59"/>
-      <c r="AG36" s="59"/>
+      <c r="AD36" s="45"/>
+      <c r="AE36" s="45"/>
+      <c r="AF36" s="45"/>
+      <c r="AG36" s="45"/>
     </row>
     <row r="37" spans="5:33" x14ac:dyDescent="0.3">
-      <c r="J37" s="59"/>
-      <c r="K37" s="59"/>
-      <c r="L37" s="59"/>
-      <c r="M37" s="59"/>
-      <c r="N37" s="59"/>
-      <c r="O37" s="59"/>
-      <c r="P37" s="59"/>
-      <c r="Q37" s="59"/>
-      <c r="R37" s="59"/>
-      <c r="V37" s="59"/>
-      <c r="W37" s="59"/>
-      <c r="X37" s="59"/>
-      <c r="Y37" s="59"/>
-      <c r="Z37" s="59"/>
-      <c r="AC37" s="59"/>
-      <c r="AD37" s="59"/>
-      <c r="AE37" s="59"/>
-      <c r="AF37" s="59"/>
-      <c r="AG37" s="59"/>
+      <c r="J37" s="45"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="45"/>
+      <c r="M37" s="45"/>
+      <c r="N37" s="45"/>
+      <c r="O37" s="45"/>
+      <c r="P37" s="45"/>
+      <c r="Q37" s="45"/>
+      <c r="R37" s="45"/>
+      <c r="V37" s="45"/>
+      <c r="W37" s="45"/>
+      <c r="X37" s="45"/>
+      <c r="Y37" s="45"/>
+      <c r="Z37" s="45"/>
+      <c r="AC37" s="45"/>
+      <c r="AD37" s="45"/>
+      <c r="AE37" s="45"/>
+      <c r="AF37" s="45"/>
+      <c r="AG37" s="45"/>
     </row>
     <row r="42" spans="5:33" x14ac:dyDescent="0.3">
       <c r="F42" s="2"/>
@@ -2611,36 +2611,6 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="AC36:AF37"/>
-    <mergeCell ref="AG36:AG37"/>
-    <mergeCell ref="J36:M37"/>
-    <mergeCell ref="N36:Q37"/>
-    <mergeCell ref="R36:R37"/>
-    <mergeCell ref="V36:Y37"/>
-    <mergeCell ref="Z36:Z37"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="C20:C21"/>
@@ -2657,6 +2627,36 @@
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="AC36:AF37"/>
+    <mergeCell ref="AG36:AG37"/>
+    <mergeCell ref="J36:M37"/>
+    <mergeCell ref="N36:Q37"/>
+    <mergeCell ref="R36:R37"/>
+    <mergeCell ref="V36:Y37"/>
+    <mergeCell ref="Z36:Z37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
playback scene with two modes working without timers. there still are error messages
</commit_message>
<xml_diff>
--- a/docs/Kinetoscope_TB_planning.xlsx
+++ b/docs/Kinetoscope_TB_planning.xlsx
@@ -161,7 +161,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,6 +192,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="33">
     <border>
@@ -653,7 +659,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -750,6 +756,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1057,7 +1067,7 @@
   <dimension ref="A1:AM45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1321,7 +1331,7 @@
       <c r="C5" s="54"/>
       <c r="D5" s="12"/>
       <c r="E5" s="43"/>
-      <c r="F5" s="23"/>
+      <c r="F5" s="62"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
       <c r="I5" s="29"/>
@@ -1669,7 +1679,7 @@
       <c r="C13" s="57"/>
       <c r="D13" s="12"/>
       <c r="E13" s="29"/>
-      <c r="F13" s="23"/>
+      <c r="F13" s="62"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="29"/>
@@ -1757,7 +1767,7 @@
       <c r="C15" s="57"/>
       <c r="D15" s="12"/>
       <c r="E15" s="29"/>
-      <c r="F15" s="23"/>
+      <c r="F15" s="62"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
       <c r="I15" s="29"/>
@@ -2365,9 +2375,9 @@
       <c r="A29" s="51"/>
       <c r="B29" s="46"/>
       <c r="C29" s="53"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="22"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="65"/>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
       <c r="I29" s="27"/>

</xml_diff>

<commit_message>
IDLE animation completed with waiting time between two replay and time to wait before replay and two possible modes
</commit_message>
<xml_diff>
--- a/docs/Kinetoscope_TB_planning.xlsx
+++ b/docs/Kinetoscope_TB_planning.xlsx
@@ -161,7 +161,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,6 +198,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="33">
     <border>
@@ -659,7 +671,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -705,19 +717,42 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -729,37 +764,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1067,7 +1083,7 @@
   <dimension ref="A1:AM45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1076,10 +1092,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="61"/>
+      <c r="B1" s="50"/>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1193,13 +1209,13 @@
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="55">
+      <c r="B2" s="54">
         <v>1</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="53" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="4"/>
@@ -1240,9 +1256,9 @@
       <c r="AM2" s="6"/>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A3" s="51"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="53"/>
+      <c r="A3" s="62"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="51"/>
       <c r="D3" s="42"/>
       <c r="E3" s="44"/>
       <c r="F3" s="22"/>
@@ -1281,11 +1297,11 @@
       <c r="AM3" s="9"/>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="46">
+      <c r="A4" s="62"/>
+      <c r="B4" s="55">
         <v>2</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="51" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="10"/>
@@ -1326,12 +1342,12 @@
       <c r="AM4" s="9"/>
     </row>
     <row r="5" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="52"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="54"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="52"/>
       <c r="D5" s="12"/>
       <c r="E5" s="43"/>
-      <c r="F5" s="62"/>
+      <c r="F5" s="45"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
       <c r="I5" s="29"/>
@@ -1367,13 +1383,13 @@
       <c r="AM5" s="14"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="55">
+      <c r="B6" s="54">
         <v>1</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="C6" s="53" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="15"/>
@@ -1414,9 +1430,9 @@
       <c r="AM6" s="6"/>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A7" s="51"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="53"/>
+      <c r="A7" s="62"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="51"/>
       <c r="D7" s="7"/>
       <c r="E7" s="44"/>
       <c r="F7" s="22"/>
@@ -1455,11 +1471,11 @@
       <c r="AM7" s="9"/>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A8" s="51"/>
-      <c r="B8" s="46">
+      <c r="A8" s="62"/>
+      <c r="B8" s="55">
         <v>2</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="51" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="7"/>
@@ -1500,9 +1516,9 @@
       <c r="AM8" s="9"/>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A9" s="51"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="53"/>
+      <c r="A9" s="62"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="51"/>
       <c r="D9" s="7"/>
       <c r="E9" s="44"/>
       <c r="F9" s="22"/>
@@ -1541,11 +1557,11 @@
       <c r="AM9" s="9"/>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A10" s="51"/>
-      <c r="B10" s="46">
+      <c r="A10" s="62"/>
+      <c r="B10" s="55">
         <v>3</v>
       </c>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="51" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="7"/>
@@ -1586,9 +1602,9 @@
       <c r="AM10" s="9"/>
     </row>
     <row r="11" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="52"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="54"/>
+      <c r="A11" s="63"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="52"/>
       <c r="D11" s="12"/>
       <c r="E11" s="43"/>
       <c r="F11" s="23"/>
@@ -1627,10 +1643,10 @@
       <c r="AM11" s="14"/>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A12" s="59" t="s">
+      <c r="A12" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="48">
+      <c r="B12" s="58">
         <v>1</v>
       </c>
       <c r="C12" s="56" t="s">
@@ -1674,12 +1690,12 @@
       <c r="AM12" s="6"/>
     </row>
     <row r="13" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="60"/>
-      <c r="B13" s="49"/>
+      <c r="A13" s="65"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="57"/>
       <c r="D13" s="12"/>
       <c r="E13" s="29"/>
-      <c r="F13" s="62"/>
+      <c r="F13" s="45"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="29"/>
@@ -1715,10 +1731,10 @@
       <c r="AM13" s="14"/>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A14" s="59" t="s">
+      <c r="A14" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="48">
+      <c r="B14" s="58">
         <v>1</v>
       </c>
       <c r="C14" s="56" t="s">
@@ -1762,15 +1778,15 @@
       <c r="AM14" s="6"/>
     </row>
     <row r="15" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="60"/>
-      <c r="B15" s="49"/>
+      <c r="A15" s="65"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="57"/>
       <c r="D15" s="12"/>
       <c r="E15" s="29"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="29"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="43"/>
       <c r="J15" s="23"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
@@ -1803,13 +1819,13 @@
       <c r="AM15" s="14"/>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A16" s="50" t="s">
+      <c r="A16" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="55">
+      <c r="B16" s="54">
         <v>1</v>
       </c>
-      <c r="C16" s="58" t="s">
+      <c r="C16" s="53" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="15"/>
@@ -1850,16 +1866,16 @@
       <c r="AM16" s="6"/>
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A17" s="51"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="53"/>
+      <c r="A17" s="62"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="51"/>
       <c r="D17" s="7"/>
       <c r="E17" s="27"/>
       <c r="F17" s="22"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="27"/>
-      <c r="J17" s="22"/>
+      <c r="J17" s="69"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
       <c r="M17" s="27"/>
@@ -1891,11 +1907,11 @@
       <c r="AM17" s="9"/>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A18" s="51"/>
-      <c r="B18" s="46">
+      <c r="A18" s="62"/>
+      <c r="B18" s="55">
         <v>2</v>
       </c>
-      <c r="C18" s="53" t="s">
+      <c r="C18" s="51" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="7"/>
@@ -1936,9 +1952,9 @@
       <c r="AM18" s="9"/>
     </row>
     <row r="19" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="52"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="54"/>
+      <c r="A19" s="63"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="52"/>
       <c r="D19" s="12"/>
       <c r="E19" s="29"/>
       <c r="F19" s="23"/>
@@ -1977,13 +1993,13 @@
       <c r="AM19" s="14"/>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="55">
+      <c r="B20" s="54">
         <v>1</v>
       </c>
-      <c r="C20" s="58" t="s">
+      <c r="C20" s="53" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="15"/>
@@ -2024,9 +2040,9 @@
       <c r="AM20" s="6"/>
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A21" s="51"/>
-      <c r="B21" s="46"/>
-      <c r="C21" s="53"/>
+      <c r="A21" s="62"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="51"/>
       <c r="D21" s="7"/>
       <c r="E21" s="27"/>
       <c r="F21" s="22"/>
@@ -2065,11 +2081,11 @@
       <c r="AM21" s="9"/>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A22" s="51"/>
-      <c r="B22" s="46">
+      <c r="A22" s="62"/>
+      <c r="B22" s="55">
         <v>2</v>
       </c>
-      <c r="C22" s="53" t="s">
+      <c r="C22" s="51" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="7"/>
@@ -2110,9 +2126,9 @@
       <c r="AM22" s="9"/>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A23" s="51"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="53"/>
+      <c r="A23" s="62"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="51"/>
       <c r="D23" s="7"/>
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
@@ -2151,11 +2167,11 @@
       <c r="AM23" s="9"/>
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A24" s="51"/>
-      <c r="B24" s="46">
+      <c r="A24" s="62"/>
+      <c r="B24" s="55">
         <v>3</v>
       </c>
-      <c r="C24" s="53" t="s">
+      <c r="C24" s="51" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="7"/>
@@ -2196,9 +2212,9 @@
       <c r="AM24" s="9"/>
     </row>
     <row r="25" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="52"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="54"/>
+      <c r="A25" s="63"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="52"/>
       <c r="D25" s="12"/>
       <c r="E25" s="29"/>
       <c r="F25" s="23"/>
@@ -2237,10 +2253,10 @@
       <c r="AM25" s="14"/>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A26" s="59" t="s">
+      <c r="A26" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="48">
+      <c r="B26" s="58">
         <v>1</v>
       </c>
       <c r="C26" s="56" t="s">
@@ -2284,8 +2300,8 @@
       <c r="AM26" s="20"/>
     </row>
     <row r="27" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="60"/>
-      <c r="B27" s="49"/>
+      <c r="A27" s="65"/>
+      <c r="B27" s="59"/>
       <c r="C27" s="57"/>
       <c r="D27" s="12"/>
       <c r="E27" s="29"/>
@@ -2325,13 +2341,13 @@
       <c r="AM27" s="14"/>
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="55">
+      <c r="B28" s="54">
         <v>1</v>
       </c>
-      <c r="C28" s="58" t="s">
+      <c r="C28" s="53" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="17"/>
@@ -2372,15 +2388,15 @@
       <c r="AM28" s="6"/>
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A29" s="51"/>
-      <c r="B29" s="46"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="63"/>
-      <c r="E29" s="64"/>
-      <c r="F29" s="65"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="27"/>
+      <c r="A29" s="62"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="68"/>
       <c r="J29" s="22"/>
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
@@ -2413,11 +2429,11 @@
       <c r="AM29" s="9"/>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A30" s="51"/>
-      <c r="B30" s="46">
+      <c r="A30" s="62"/>
+      <c r="B30" s="55">
         <v>2</v>
       </c>
-      <c r="C30" s="53" t="s">
+      <c r="C30" s="51" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="7"/>
@@ -2458,9 +2474,9 @@
       <c r="AM30" s="19"/>
     </row>
     <row r="31" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="52"/>
-      <c r="B31" s="47"/>
-      <c r="C31" s="54"/>
+      <c r="A31" s="63"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="52"/>
       <c r="D31" s="12"/>
       <c r="E31" s="29"/>
       <c r="F31" s="23"/>
@@ -2546,54 +2562,54 @@
         <v>27</v>
       </c>
       <c r="G36" s="34"/>
-      <c r="J36" s="45" t="s">
+      <c r="J36" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45" t="s">
+      <c r="K36" s="66"/>
+      <c r="L36" s="66"/>
+      <c r="M36" s="66"/>
+      <c r="N36" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="45"/>
-      <c r="R36" s="45"/>
-      <c r="V36" s="45" t="s">
+      <c r="O36" s="66"/>
+      <c r="P36" s="66"/>
+      <c r="Q36" s="66"/>
+      <c r="R36" s="66"/>
+      <c r="V36" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="W36" s="45"/>
-      <c r="X36" s="45"/>
-      <c r="Y36" s="45"/>
-      <c r="Z36" s="45"/>
-      <c r="AC36" s="45" t="s">
+      <c r="W36" s="66"/>
+      <c r="X36" s="66"/>
+      <c r="Y36" s="66"/>
+      <c r="Z36" s="66"/>
+      <c r="AC36" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="AD36" s="45"/>
-      <c r="AE36" s="45"/>
-      <c r="AF36" s="45"/>
-      <c r="AG36" s="45"/>
+      <c r="AD36" s="66"/>
+      <c r="AE36" s="66"/>
+      <c r="AF36" s="66"/>
+      <c r="AG36" s="66"/>
     </row>
     <row r="37" spans="5:33" x14ac:dyDescent="0.3">
-      <c r="J37" s="45"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="45"/>
-      <c r="M37" s="45"/>
-      <c r="N37" s="45"/>
-      <c r="O37" s="45"/>
-      <c r="P37" s="45"/>
-      <c r="Q37" s="45"/>
-      <c r="R37" s="45"/>
-      <c r="V37" s="45"/>
-      <c r="W37" s="45"/>
-      <c r="X37" s="45"/>
-      <c r="Y37" s="45"/>
-      <c r="Z37" s="45"/>
-      <c r="AC37" s="45"/>
-      <c r="AD37" s="45"/>
-      <c r="AE37" s="45"/>
-      <c r="AF37" s="45"/>
-      <c r="AG37" s="45"/>
+      <c r="J37" s="66"/>
+      <c r="K37" s="66"/>
+      <c r="L37" s="66"/>
+      <c r="M37" s="66"/>
+      <c r="N37" s="66"/>
+      <c r="O37" s="66"/>
+      <c r="P37" s="66"/>
+      <c r="Q37" s="66"/>
+      <c r="R37" s="66"/>
+      <c r="V37" s="66"/>
+      <c r="W37" s="66"/>
+      <c r="X37" s="66"/>
+      <c r="Y37" s="66"/>
+      <c r="Z37" s="66"/>
+      <c r="AC37" s="66"/>
+      <c r="AD37" s="66"/>
+      <c r="AE37" s="66"/>
+      <c r="AF37" s="66"/>
+      <c r="AG37" s="66"/>
     </row>
     <row r="42" spans="5:33" x14ac:dyDescent="0.3">
       <c r="F42" s="2"/>
@@ -2621,6 +2637,36 @@
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="AC36:AF37"/>
+    <mergeCell ref="AG36:AG37"/>
+    <mergeCell ref="J36:M37"/>
+    <mergeCell ref="N36:Q37"/>
+    <mergeCell ref="R36:R37"/>
+    <mergeCell ref="V36:Y37"/>
+    <mergeCell ref="Z36:Z37"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="C20:C21"/>
@@ -2637,36 +2683,6 @@
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="AC36:AF37"/>
-    <mergeCell ref="AG36:AG37"/>
-    <mergeCell ref="J36:M37"/>
-    <mergeCell ref="N36:Q37"/>
-    <mergeCell ref="R36:R37"/>
-    <mergeCell ref="V36:Y37"/>
-    <mergeCell ref="Z36:Z37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Network first version of unity server and connexion script
</commit_message>
<xml_diff>
--- a/docs/Kinetoscope_TB_planning.xlsx
+++ b/docs/Kinetoscope_TB_planning.xlsx
@@ -144,7 +144,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,8 +160,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,6 +213,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -671,7 +684,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -775,7 +788,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1083,7 +1097,7 @@
   <dimension ref="A1:AM45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1783,7 +1797,7 @@
       <c r="C15" s="57"/>
       <c r="D15" s="12"/>
       <c r="E15" s="29"/>
-      <c r="F15" s="45"/>
+      <c r="F15" s="69"/>
       <c r="G15" s="49"/>
       <c r="H15" s="49"/>
       <c r="I15" s="43"/>
@@ -1875,7 +1889,7 @@
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="27"/>
-      <c r="J17" s="69"/>
+      <c r="J17" s="70"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
       <c r="M17" s="27"/>
@@ -2685,7 +2699,7 @@
     <mergeCell ref="C14:C15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
first try with a networkView object updated through network
</commit_message>
<xml_diff>
--- a/docs/Kinetoscope_TB_planning.xlsx
+++ b/docs/Kinetoscope_TB_planning.xlsx
@@ -684,7 +684,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -735,37 +735,23 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -777,19 +763,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1097,7 +1098,7 @@
   <dimension ref="A1:AM45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1106,10 +1107,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
+      <c r="B1" s="70"/>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1223,13 +1224,13 @@
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="54">
+      <c r="B2" s="64">
         <v>1</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="67" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="4"/>
@@ -1270,9 +1271,9 @@
       <c r="AM2" s="6"/>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A3" s="62"/>
+      <c r="A3" s="60"/>
       <c r="B3" s="55"/>
-      <c r="C3" s="51"/>
+      <c r="C3" s="62"/>
       <c r="D3" s="42"/>
       <c r="E3" s="44"/>
       <c r="F3" s="22"/>
@@ -1311,11 +1312,11 @@
       <c r="AM3" s="9"/>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A4" s="62"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="55">
         <v>2</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="62" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="10"/>
@@ -1356,9 +1357,9 @@
       <c r="AM4" s="9"/>
     </row>
     <row r="5" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="63"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="52"/>
+      <c r="A5" s="61"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="63"/>
       <c r="D5" s="12"/>
       <c r="E5" s="43"/>
       <c r="F5" s="45"/>
@@ -1397,13 +1398,13 @@
       <c r="AM5" s="14"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="54">
+      <c r="B6" s="64">
         <v>1</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="67" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="15"/>
@@ -1444,9 +1445,9 @@
       <c r="AM6" s="6"/>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A7" s="62"/>
+      <c r="A7" s="60"/>
       <c r="B7" s="55"/>
-      <c r="C7" s="51"/>
+      <c r="C7" s="62"/>
       <c r="D7" s="7"/>
       <c r="E7" s="44"/>
       <c r="F7" s="22"/>
@@ -1485,11 +1486,11 @@
       <c r="AM7" s="9"/>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A8" s="62"/>
+      <c r="A8" s="60"/>
       <c r="B8" s="55">
         <v>2</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="62" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="7"/>
@@ -1530,9 +1531,9 @@
       <c r="AM8" s="9"/>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A9" s="62"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="55"/>
-      <c r="C9" s="51"/>
+      <c r="C9" s="62"/>
       <c r="D9" s="7"/>
       <c r="E9" s="44"/>
       <c r="F9" s="22"/>
@@ -1571,11 +1572,11 @@
       <c r="AM9" s="9"/>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A10" s="62"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="55">
         <v>3</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="C10" s="62" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="7"/>
@@ -1616,9 +1617,9 @@
       <c r="AM10" s="9"/>
     </row>
     <row r="11" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="63"/>
-      <c r="B11" s="60"/>
-      <c r="C11" s="52"/>
+      <c r="A11" s="61"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="63"/>
       <c r="D11" s="12"/>
       <c r="E11" s="43"/>
       <c r="F11" s="23"/>
@@ -1657,13 +1658,13 @@
       <c r="AM11" s="14"/>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="58">
+      <c r="B12" s="57">
         <v>1</v>
       </c>
-      <c r="C12" s="56" t="s">
+      <c r="C12" s="65" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="15"/>
@@ -1704,9 +1705,9 @@
       <c r="AM12" s="6"/>
     </row>
     <row r="13" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="65"/>
-      <c r="B13" s="59"/>
-      <c r="C13" s="57"/>
+      <c r="A13" s="69"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="66"/>
       <c r="D13" s="12"/>
       <c r="E13" s="29"/>
       <c r="F13" s="45"/>
@@ -1745,13 +1746,13 @@
       <c r="AM13" s="14"/>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A14" s="64" t="s">
+      <c r="A14" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="58">
+      <c r="B14" s="57">
         <v>1</v>
       </c>
-      <c r="C14" s="56" t="s">
+      <c r="C14" s="65" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="15"/>
@@ -1792,12 +1793,12 @@
       <c r="AM14" s="6"/>
     </row>
     <row r="15" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="65"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="57"/>
+      <c r="A15" s="69"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="66"/>
       <c r="D15" s="12"/>
       <c r="E15" s="29"/>
-      <c r="F15" s="69"/>
+      <c r="F15" s="52"/>
       <c r="G15" s="49"/>
       <c r="H15" s="49"/>
       <c r="I15" s="43"/>
@@ -1833,13 +1834,13 @@
       <c r="AM15" s="14"/>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A16" s="61" t="s">
+      <c r="A16" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="54">
+      <c r="B16" s="64">
         <v>1</v>
       </c>
-      <c r="C16" s="53" t="s">
+      <c r="C16" s="67" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="15"/>
@@ -1880,18 +1881,18 @@
       <c r="AM16" s="6"/>
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A17" s="62"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="55"/>
-      <c r="C17" s="51"/>
+      <c r="C17" s="62"/>
       <c r="D17" s="7"/>
       <c r="E17" s="27"/>
       <c r="F17" s="22"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="27"/>
-      <c r="J17" s="70"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="71"/>
       <c r="M17" s="27"/>
       <c r="N17" s="22"/>
       <c r="O17" s="36"/>
@@ -1921,11 +1922,11 @@
       <c r="AM17" s="9"/>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A18" s="62"/>
+      <c r="A18" s="60"/>
       <c r="B18" s="55">
         <v>2</v>
       </c>
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="62" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="7"/>
@@ -1966,9 +1967,9 @@
       <c r="AM18" s="9"/>
     </row>
     <row r="19" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="63"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="52"/>
+      <c r="A19" s="61"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="63"/>
       <c r="D19" s="12"/>
       <c r="E19" s="29"/>
       <c r="F19" s="23"/>
@@ -1977,7 +1978,7 @@
       <c r="I19" s="29"/>
       <c r="J19" s="23"/>
       <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
+      <c r="L19" s="49"/>
       <c r="M19" s="29"/>
       <c r="N19" s="23"/>
       <c r="O19" s="37"/>
@@ -2007,13 +2008,13 @@
       <c r="AM19" s="14"/>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A20" s="61" t="s">
+      <c r="A20" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="54">
+      <c r="B20" s="64">
         <v>1</v>
       </c>
-      <c r="C20" s="53" t="s">
+      <c r="C20" s="67" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="15"/>
@@ -2054,9 +2055,9 @@
       <c r="AM20" s="6"/>
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A21" s="62"/>
+      <c r="A21" s="60"/>
       <c r="B21" s="55"/>
-      <c r="C21" s="51"/>
+      <c r="C21" s="62"/>
       <c r="D21" s="7"/>
       <c r="E21" s="27"/>
       <c r="F21" s="22"/>
@@ -2095,11 +2096,11 @@
       <c r="AM21" s="9"/>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A22" s="62"/>
+      <c r="A22" s="60"/>
       <c r="B22" s="55">
         <v>2</v>
       </c>
-      <c r="C22" s="51" t="s">
+      <c r="C22" s="62" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="7"/>
@@ -2140,9 +2141,9 @@
       <c r="AM22" s="9"/>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A23" s="62"/>
+      <c r="A23" s="60"/>
       <c r="B23" s="55"/>
-      <c r="C23" s="51"/>
+      <c r="C23" s="62"/>
       <c r="D23" s="7"/>
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
@@ -2181,11 +2182,11 @@
       <c r="AM23" s="9"/>
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A24" s="62"/>
+      <c r="A24" s="60"/>
       <c r="B24" s="55">
         <v>3</v>
       </c>
-      <c r="C24" s="51" t="s">
+      <c r="C24" s="62" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="7"/>
@@ -2226,9 +2227,9 @@
       <c r="AM24" s="9"/>
     </row>
     <row r="25" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="63"/>
-      <c r="B25" s="60"/>
-      <c r="C25" s="52"/>
+      <c r="A25" s="61"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="63"/>
       <c r="D25" s="12"/>
       <c r="E25" s="29"/>
       <c r="F25" s="23"/>
@@ -2267,13 +2268,13 @@
       <c r="AM25" s="14"/>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A26" s="64" t="s">
+      <c r="A26" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="58">
+      <c r="B26" s="57">
         <v>1</v>
       </c>
-      <c r="C26" s="56" t="s">
+      <c r="C26" s="65" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="15"/>
@@ -2314,9 +2315,9 @@
       <c r="AM26" s="20"/>
     </row>
     <row r="27" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="65"/>
-      <c r="B27" s="59"/>
-      <c r="C27" s="57"/>
+      <c r="A27" s="69"/>
+      <c r="B27" s="58"/>
+      <c r="C27" s="66"/>
       <c r="D27" s="12"/>
       <c r="E27" s="29"/>
       <c r="F27" s="23"/>
@@ -2355,13 +2356,13 @@
       <c r="AM27" s="14"/>
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A28" s="61" t="s">
+      <c r="A28" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="54">
+      <c r="B28" s="64">
         <v>1</v>
       </c>
-      <c r="C28" s="53" t="s">
+      <c r="C28" s="67" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="17"/>
@@ -2402,15 +2403,15 @@
       <c r="AM28" s="6"/>
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A29" s="62"/>
+      <c r="A29" s="60"/>
       <c r="B29" s="55"/>
-      <c r="C29" s="51"/>
+      <c r="C29" s="62"/>
       <c r="D29" s="46"/>
       <c r="E29" s="47"/>
       <c r="F29" s="48"/>
-      <c r="G29" s="67"/>
-      <c r="H29" s="67"/>
-      <c r="I29" s="68"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="51"/>
       <c r="J29" s="22"/>
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
@@ -2443,11 +2444,11 @@
       <c r="AM29" s="9"/>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A30" s="62"/>
+      <c r="A30" s="60"/>
       <c r="B30" s="55">
         <v>2</v>
       </c>
-      <c r="C30" s="51" t="s">
+      <c r="C30" s="62" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="7"/>
@@ -2488,9 +2489,9 @@
       <c r="AM30" s="19"/>
     </row>
     <row r="31" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="63"/>
-      <c r="B31" s="60"/>
-      <c r="C31" s="52"/>
+      <c r="A31" s="61"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="63"/>
       <c r="D31" s="12"/>
       <c r="E31" s="29"/>
       <c r="F31" s="23"/>
@@ -2576,54 +2577,54 @@
         <v>27</v>
       </c>
       <c r="G36" s="34"/>
-      <c r="J36" s="66" t="s">
+      <c r="J36" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="K36" s="66"/>
-      <c r="L36" s="66"/>
-      <c r="M36" s="66"/>
-      <c r="N36" s="66" t="s">
+      <c r="K36" s="54"/>
+      <c r="L36" s="54"/>
+      <c r="M36" s="54"/>
+      <c r="N36" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="O36" s="66"/>
-      <c r="P36" s="66"/>
-      <c r="Q36" s="66"/>
-      <c r="R36" s="66"/>
-      <c r="V36" s="66" t="s">
+      <c r="O36" s="54"/>
+      <c r="P36" s="54"/>
+      <c r="Q36" s="54"/>
+      <c r="R36" s="54"/>
+      <c r="V36" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="W36" s="66"/>
-      <c r="X36" s="66"/>
-      <c r="Y36" s="66"/>
-      <c r="Z36" s="66"/>
-      <c r="AC36" s="66" t="s">
+      <c r="W36" s="54"/>
+      <c r="X36" s="54"/>
+      <c r="Y36" s="54"/>
+      <c r="Z36" s="54"/>
+      <c r="AC36" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="AD36" s="66"/>
-      <c r="AE36" s="66"/>
-      <c r="AF36" s="66"/>
-      <c r="AG36" s="66"/>
+      <c r="AD36" s="54"/>
+      <c r="AE36" s="54"/>
+      <c r="AF36" s="54"/>
+      <c r="AG36" s="54"/>
     </row>
     <row r="37" spans="5:33" x14ac:dyDescent="0.3">
-      <c r="J37" s="66"/>
-      <c r="K37" s="66"/>
-      <c r="L37" s="66"/>
-      <c r="M37" s="66"/>
-      <c r="N37" s="66"/>
-      <c r="O37" s="66"/>
-      <c r="P37" s="66"/>
-      <c r="Q37" s="66"/>
-      <c r="R37" s="66"/>
-      <c r="V37" s="66"/>
-      <c r="W37" s="66"/>
-      <c r="X37" s="66"/>
-      <c r="Y37" s="66"/>
-      <c r="Z37" s="66"/>
-      <c r="AC37" s="66"/>
-      <c r="AD37" s="66"/>
-      <c r="AE37" s="66"/>
-      <c r="AF37" s="66"/>
-      <c r="AG37" s="66"/>
+      <c r="J37" s="54"/>
+      <c r="K37" s="54"/>
+      <c r="L37" s="54"/>
+      <c r="M37" s="54"/>
+      <c r="N37" s="54"/>
+      <c r="O37" s="54"/>
+      <c r="P37" s="54"/>
+      <c r="Q37" s="54"/>
+      <c r="R37" s="54"/>
+      <c r="V37" s="54"/>
+      <c r="W37" s="54"/>
+      <c r="X37" s="54"/>
+      <c r="Y37" s="54"/>
+      <c r="Z37" s="54"/>
+      <c r="AC37" s="54"/>
+      <c r="AD37" s="54"/>
+      <c r="AE37" s="54"/>
+      <c r="AF37" s="54"/>
+      <c r="AG37" s="54"/>
     </row>
     <row r="42" spans="5:33" x14ac:dyDescent="0.3">
       <c r="F42" s="2"/>
@@ -2651,36 +2652,6 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="AC36:AF37"/>
-    <mergeCell ref="AG36:AG37"/>
-    <mergeCell ref="J36:M37"/>
-    <mergeCell ref="N36:Q37"/>
-    <mergeCell ref="R36:R37"/>
-    <mergeCell ref="V36:Y37"/>
-    <mergeCell ref="Z36:Z37"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="C20:C21"/>
@@ -2697,6 +2668,36 @@
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="AC36:AF37"/>
+    <mergeCell ref="AG36:AG37"/>
+    <mergeCell ref="J36:M37"/>
+    <mergeCell ref="N36:Q37"/>
+    <mergeCell ref="R36:R37"/>
+    <mergeCell ref="V36:Y37"/>
+    <mergeCell ref="Z36:Z37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
flickr effect functionnal and deploy bug fixed
</commit_message>
<xml_diff>
--- a/docs/Kinetoscope_TB_planning.xlsx
+++ b/docs/Kinetoscope_TB_planning.xlsx
@@ -684,7 +684,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -791,6 +791,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1098,7 +1101,7 @@
   <dimension ref="A1:AM45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1893,7 +1896,7 @@
       <c r="J17" s="53"/>
       <c r="K17" s="71"/>
       <c r="L17" s="71"/>
-      <c r="M17" s="27"/>
+      <c r="M17" s="44"/>
       <c r="N17" s="22"/>
       <c r="O17" s="36"/>
       <c r="P17" s="36"/>
@@ -1978,8 +1981,8 @@
       <c r="I19" s="29"/>
       <c r="J19" s="23"/>
       <c r="K19" s="13"/>
-      <c r="L19" s="49"/>
-      <c r="M19" s="29"/>
+      <c r="L19" s="72"/>
+      <c r="M19" s="43"/>
       <c r="N19" s="23"/>
       <c r="O19" s="37"/>
       <c r="P19" s="37"/>
@@ -2068,7 +2071,7 @@
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
       <c r="M21" s="27"/>
-      <c r="N21" s="22"/>
+      <c r="N21" s="73"/>
       <c r="O21" s="36"/>
       <c r="P21" s="36"/>
       <c r="Q21" s="36"/>
@@ -2412,7 +2415,7 @@
       <c r="G29" s="50"/>
       <c r="H29" s="50"/>
       <c r="I29" s="51"/>
-      <c r="J29" s="22"/>
+      <c r="J29" s="74"/>
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
       <c r="M29" s="27"/>

</xml_diff>

<commit_message>
project clean and planning update
</commit_message>
<xml_diff>
--- a/docs/Kinetoscope_TB_planning.xlsx
+++ b/docs/Kinetoscope_TB_planning.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kilian.brandtdi\Documents\Visual Studio 2013\xvision\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="768" yWindow="336" windowWidth="21828" windowHeight="9264"/>
   </bookViews>
@@ -684,7 +679,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -739,19 +734,40 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -763,37 +779,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -854,7 +855,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -889,7 +890,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1098,10 +1099,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:AM45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+      <selection activeCell="AE15" sqref="AE15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1110,10 +1114,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
+      <c r="B1" s="57"/>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1227,13 +1231,13 @@
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="64">
+      <c r="B2" s="61">
         <v>1</v>
       </c>
-      <c r="C2" s="67" t="s">
+      <c r="C2" s="60" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="4"/>
@@ -1250,7 +1254,7 @@
       <c r="O2" s="35"/>
       <c r="P2" s="35"/>
       <c r="Q2" s="35"/>
-      <c r="R2" s="5"/>
+      <c r="R2" s="35"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
       <c r="U2" s="26"/>
@@ -1274,9 +1278,9 @@
       <c r="AM2" s="6"/>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A3" s="60"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="62"/>
+      <c r="A3" s="69"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="58"/>
       <c r="D3" s="42"/>
       <c r="E3" s="44"/>
       <c r="F3" s="22"/>
@@ -1291,7 +1295,7 @@
       <c r="O3" s="36"/>
       <c r="P3" s="36"/>
       <c r="Q3" s="36"/>
-      <c r="R3" s="8"/>
+      <c r="R3" s="36"/>
       <c r="S3" s="8"/>
       <c r="T3" s="8"/>
       <c r="U3" s="27"/>
@@ -1315,11 +1319,11 @@
       <c r="AM3" s="9"/>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A4" s="60"/>
-      <c r="B4" s="55">
+      <c r="A4" s="69"/>
+      <c r="B4" s="62">
         <v>2</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="58" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="10"/>
@@ -1336,7 +1340,7 @@
       <c r="O4" s="36"/>
       <c r="P4" s="36"/>
       <c r="Q4" s="36"/>
-      <c r="R4" s="8"/>
+      <c r="R4" s="36"/>
       <c r="S4" s="8"/>
       <c r="T4" s="8"/>
       <c r="U4" s="27"/>
@@ -1360,9 +1364,9 @@
       <c r="AM4" s="9"/>
     </row>
     <row r="5" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="61"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="63"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="12"/>
       <c r="E5" s="43"/>
       <c r="F5" s="45"/>
@@ -1377,7 +1381,7 @@
       <c r="O5" s="37"/>
       <c r="P5" s="37"/>
       <c r="Q5" s="37"/>
-      <c r="R5" s="13"/>
+      <c r="R5" s="37"/>
       <c r="S5" s="13"/>
       <c r="T5" s="13"/>
       <c r="U5" s="29"/>
@@ -1401,13 +1405,13 @@
       <c r="AM5" s="14"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="64">
+      <c r="B6" s="61">
         <v>1</v>
       </c>
-      <c r="C6" s="67" t="s">
+      <c r="C6" s="60" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="15"/>
@@ -1424,7 +1428,7 @@
       <c r="O6" s="35"/>
       <c r="P6" s="35"/>
       <c r="Q6" s="35"/>
-      <c r="R6" s="5"/>
+      <c r="R6" s="35"/>
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
       <c r="U6" s="26"/>
@@ -1448,9 +1452,9 @@
       <c r="AM6" s="6"/>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A7" s="60"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="62"/>
+      <c r="A7" s="69"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="58"/>
       <c r="D7" s="7"/>
       <c r="E7" s="44"/>
       <c r="F7" s="22"/>
@@ -1465,7 +1469,7 @@
       <c r="O7" s="36"/>
       <c r="P7" s="36"/>
       <c r="Q7" s="36"/>
-      <c r="R7" s="8"/>
+      <c r="R7" s="36"/>
       <c r="S7" s="8"/>
       <c r="T7" s="8"/>
       <c r="U7" s="27"/>
@@ -1489,11 +1493,11 @@
       <c r="AM7" s="9"/>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A8" s="60"/>
-      <c r="B8" s="55">
+      <c r="A8" s="69"/>
+      <c r="B8" s="62">
         <v>2</v>
       </c>
-      <c r="C8" s="62" t="s">
+      <c r="C8" s="58" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="7"/>
@@ -1510,7 +1514,7 @@
       <c r="O8" s="36"/>
       <c r="P8" s="36"/>
       <c r="Q8" s="36"/>
-      <c r="R8" s="8"/>
+      <c r="R8" s="36"/>
       <c r="S8" s="8"/>
       <c r="T8" s="8"/>
       <c r="U8" s="27"/>
@@ -1534,9 +1538,9 @@
       <c r="AM8" s="9"/>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A9" s="60"/>
-      <c r="B9" s="55"/>
-      <c r="C9" s="62"/>
+      <c r="A9" s="69"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="58"/>
       <c r="D9" s="7"/>
       <c r="E9" s="44"/>
       <c r="F9" s="22"/>
@@ -1551,7 +1555,7 @@
       <c r="O9" s="36"/>
       <c r="P9" s="36"/>
       <c r="Q9" s="36"/>
-      <c r="R9" s="8"/>
+      <c r="R9" s="36"/>
       <c r="S9" s="8"/>
       <c r="T9" s="8"/>
       <c r="U9" s="27"/>
@@ -1575,11 +1579,11 @@
       <c r="AM9" s="9"/>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A10" s="60"/>
-      <c r="B10" s="55">
+      <c r="A10" s="69"/>
+      <c r="B10" s="62">
         <v>3</v>
       </c>
-      <c r="C10" s="62" t="s">
+      <c r="C10" s="58" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="7"/>
@@ -1596,7 +1600,7 @@
       <c r="O10" s="36"/>
       <c r="P10" s="36"/>
       <c r="Q10" s="36"/>
-      <c r="R10" s="8"/>
+      <c r="R10" s="36"/>
       <c r="S10" s="8"/>
       <c r="T10" s="8"/>
       <c r="U10" s="27"/>
@@ -1620,9 +1624,9 @@
       <c r="AM10" s="9"/>
     </row>
     <row r="11" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="61"/>
-      <c r="B11" s="56"/>
-      <c r="C11" s="63"/>
+      <c r="A11" s="70"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="59"/>
       <c r="D11" s="12"/>
       <c r="E11" s="43"/>
       <c r="F11" s="23"/>
@@ -1637,7 +1641,7 @@
       <c r="O11" s="37"/>
       <c r="P11" s="37"/>
       <c r="Q11" s="37"/>
-      <c r="R11" s="13"/>
+      <c r="R11" s="37"/>
       <c r="S11" s="13"/>
       <c r="T11" s="13"/>
       <c r="U11" s="29"/>
@@ -1661,13 +1665,13 @@
       <c r="AM11" s="14"/>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A12" s="68" t="s">
+      <c r="A12" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="57">
+      <c r="B12" s="65">
         <v>1</v>
       </c>
-      <c r="C12" s="65" t="s">
+      <c r="C12" s="63" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="15"/>
@@ -1684,7 +1688,7 @@
       <c r="O12" s="35"/>
       <c r="P12" s="35"/>
       <c r="Q12" s="35"/>
-      <c r="R12" s="5"/>
+      <c r="R12" s="35"/>
       <c r="S12" s="5"/>
       <c r="T12" s="5"/>
       <c r="U12" s="26"/>
@@ -1708,9 +1712,9 @@
       <c r="AM12" s="6"/>
     </row>
     <row r="13" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="69"/>
-      <c r="B13" s="58"/>
-      <c r="C13" s="66"/>
+      <c r="A13" s="72"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="64"/>
       <c r="D13" s="12"/>
       <c r="E13" s="29"/>
       <c r="F13" s="45"/>
@@ -1725,11 +1729,11 @@
       <c r="O13" s="37"/>
       <c r="P13" s="37"/>
       <c r="Q13" s="37"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="13"/>
-      <c r="T13" s="13"/>
+      <c r="R13" s="37"/>
+      <c r="S13" s="49"/>
+      <c r="T13" s="49"/>
       <c r="U13" s="29"/>
-      <c r="V13" s="23"/>
+      <c r="V13" s="45"/>
       <c r="W13" s="13"/>
       <c r="X13" s="13"/>
       <c r="Y13" s="13"/>
@@ -1749,13 +1753,13 @@
       <c r="AM13" s="14"/>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A14" s="68" t="s">
+      <c r="A14" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="57">
+      <c r="B14" s="65">
         <v>1</v>
       </c>
-      <c r="C14" s="65" t="s">
+      <c r="C14" s="63" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="15"/>
@@ -1772,7 +1776,7 @@
       <c r="O14" s="35"/>
       <c r="P14" s="35"/>
       <c r="Q14" s="35"/>
-      <c r="R14" s="5"/>
+      <c r="R14" s="35"/>
       <c r="S14" s="5"/>
       <c r="T14" s="5"/>
       <c r="U14" s="26"/>
@@ -1796,9 +1800,9 @@
       <c r="AM14" s="6"/>
     </row>
     <row r="15" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="69"/>
-      <c r="B15" s="58"/>
-      <c r="C15" s="66"/>
+      <c r="A15" s="72"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="64"/>
       <c r="D15" s="12"/>
       <c r="E15" s="29"/>
       <c r="F15" s="52"/>
@@ -1813,11 +1817,11 @@
       <c r="O15" s="37"/>
       <c r="P15" s="37"/>
       <c r="Q15" s="37"/>
-      <c r="R15" s="13"/>
+      <c r="R15" s="37"/>
       <c r="S15" s="13"/>
-      <c r="T15" s="13"/>
+      <c r="T15" s="55"/>
       <c r="U15" s="29"/>
-      <c r="V15" s="23"/>
+      <c r="V15" s="45"/>
       <c r="W15" s="13"/>
       <c r="X15" s="13"/>
       <c r="Y15" s="13"/>
@@ -1837,13 +1841,13 @@
       <c r="AM15" s="14"/>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A16" s="59" t="s">
+      <c r="A16" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="64">
+      <c r="B16" s="61">
         <v>1</v>
       </c>
-      <c r="C16" s="67" t="s">
+      <c r="C16" s="60" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="15"/>
@@ -1860,7 +1864,7 @@
       <c r="O16" s="35"/>
       <c r="P16" s="35"/>
       <c r="Q16" s="35"/>
-      <c r="R16" s="5"/>
+      <c r="R16" s="35"/>
       <c r="S16" s="5"/>
       <c r="T16" s="5"/>
       <c r="U16" s="26"/>
@@ -1884,9 +1888,9 @@
       <c r="AM16" s="6"/>
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A17" s="60"/>
-      <c r="B17" s="55"/>
-      <c r="C17" s="62"/>
+      <c r="A17" s="69"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="58"/>
       <c r="D17" s="7"/>
       <c r="E17" s="27"/>
       <c r="F17" s="22"/>
@@ -1894,14 +1898,14 @@
       <c r="H17" s="8"/>
       <c r="I17" s="27"/>
       <c r="J17" s="53"/>
-      <c r="K17" s="71"/>
-      <c r="L17" s="71"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="54"/>
       <c r="M17" s="44"/>
-      <c r="N17" s="22"/>
+      <c r="N17" s="79"/>
       <c r="O17" s="36"/>
       <c r="P17" s="36"/>
       <c r="Q17" s="36"/>
-      <c r="R17" s="8"/>
+      <c r="R17" s="36"/>
       <c r="S17" s="8"/>
       <c r="T17" s="8"/>
       <c r="U17" s="27"/>
@@ -1925,11 +1929,11 @@
       <c r="AM17" s="9"/>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A18" s="60"/>
-      <c r="B18" s="55">
+      <c r="A18" s="69"/>
+      <c r="B18" s="62">
         <v>2</v>
       </c>
-      <c r="C18" s="62" t="s">
+      <c r="C18" s="58" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="7"/>
@@ -1946,7 +1950,7 @@
       <c r="O18" s="36"/>
       <c r="P18" s="36"/>
       <c r="Q18" s="36"/>
-      <c r="R18" s="8"/>
+      <c r="R18" s="36"/>
       <c r="S18" s="8"/>
       <c r="T18" s="8"/>
       <c r="U18" s="27"/>
@@ -1970,9 +1974,9 @@
       <c r="AM18" s="9"/>
     </row>
     <row r="19" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="61"/>
-      <c r="B19" s="56"/>
-      <c r="C19" s="63"/>
+      <c r="A19" s="70"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="59"/>
       <c r="D19" s="12"/>
       <c r="E19" s="29"/>
       <c r="F19" s="23"/>
@@ -1981,13 +1985,13 @@
       <c r="I19" s="29"/>
       <c r="J19" s="23"/>
       <c r="K19" s="13"/>
-      <c r="L19" s="72"/>
+      <c r="L19" s="55"/>
       <c r="M19" s="43"/>
-      <c r="N19" s="23"/>
+      <c r="N19" s="45"/>
       <c r="O19" s="37"/>
       <c r="P19" s="37"/>
       <c r="Q19" s="37"/>
-      <c r="R19" s="13"/>
+      <c r="R19" s="37"/>
       <c r="S19" s="13"/>
       <c r="T19" s="13"/>
       <c r="U19" s="29"/>
@@ -2011,13 +2015,13 @@
       <c r="AM19" s="14"/>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A20" s="59" t="s">
+      <c r="A20" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="64">
+      <c r="B20" s="61">
         <v>1</v>
       </c>
-      <c r="C20" s="67" t="s">
+      <c r="C20" s="60" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="15"/>
@@ -2034,7 +2038,7 @@
       <c r="O20" s="35"/>
       <c r="P20" s="35"/>
       <c r="Q20" s="35"/>
-      <c r="R20" s="5"/>
+      <c r="R20" s="35"/>
       <c r="S20" s="5"/>
       <c r="T20" s="5"/>
       <c r="U20" s="26"/>
@@ -2058,9 +2062,9 @@
       <c r="AM20" s="6"/>
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A21" s="60"/>
-      <c r="B21" s="55"/>
-      <c r="C21" s="62"/>
+      <c r="A21" s="69"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="58"/>
       <c r="D21" s="7"/>
       <c r="E21" s="27"/>
       <c r="F21" s="22"/>
@@ -2071,11 +2075,11 @@
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
       <c r="M21" s="27"/>
-      <c r="N21" s="73"/>
+      <c r="N21" s="56"/>
       <c r="O21" s="36"/>
       <c r="P21" s="36"/>
       <c r="Q21" s="36"/>
-      <c r="R21" s="8"/>
+      <c r="R21" s="36"/>
       <c r="S21" s="8"/>
       <c r="T21" s="8"/>
       <c r="U21" s="27"/>
@@ -2083,7 +2087,7 @@
       <c r="W21" s="8"/>
       <c r="X21" s="8"/>
       <c r="Y21" s="8"/>
-      <c r="Z21" s="8"/>
+      <c r="Z21" s="54"/>
       <c r="AA21" s="8"/>
       <c r="AB21" s="27"/>
       <c r="AC21" s="22"/>
@@ -2099,11 +2103,11 @@
       <c r="AM21" s="9"/>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A22" s="60"/>
-      <c r="B22" s="55">
+      <c r="A22" s="69"/>
+      <c r="B22" s="62">
         <v>2</v>
       </c>
-      <c r="C22" s="62" t="s">
+      <c r="C22" s="58" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="7"/>
@@ -2120,7 +2124,7 @@
       <c r="O22" s="36"/>
       <c r="P22" s="36"/>
       <c r="Q22" s="36"/>
-      <c r="R22" s="11"/>
+      <c r="R22" s="36"/>
       <c r="S22" s="11"/>
       <c r="T22" s="8"/>
       <c r="U22" s="27"/>
@@ -2144,9 +2148,9 @@
       <c r="AM22" s="9"/>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A23" s="60"/>
-      <c r="B23" s="55"/>
-      <c r="C23" s="62"/>
+      <c r="A23" s="69"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="58"/>
       <c r="D23" s="7"/>
       <c r="E23" s="27"/>
       <c r="F23" s="22"/>
@@ -2161,17 +2165,17 @@
       <c r="O23" s="36"/>
       <c r="P23" s="36"/>
       <c r="Q23" s="36"/>
-      <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
+      <c r="R23" s="36"/>
+      <c r="S23" s="54"/>
       <c r="T23" s="8"/>
       <c r="U23" s="27"/>
       <c r="V23" s="22"/>
       <c r="W23" s="8"/>
       <c r="X23" s="8"/>
-      <c r="Y23" s="8"/>
-      <c r="Z23" s="8"/>
-      <c r="AA23" s="8"/>
-      <c r="AB23" s="27"/>
+      <c r="Y23" s="74"/>
+      <c r="Z23" s="54"/>
+      <c r="AA23" s="54"/>
+      <c r="AB23" s="44"/>
       <c r="AC23" s="22"/>
       <c r="AD23" s="8"/>
       <c r="AE23" s="8"/>
@@ -2185,11 +2189,11 @@
       <c r="AM23" s="9"/>
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A24" s="60"/>
-      <c r="B24" s="55">
+      <c r="A24" s="69"/>
+      <c r="B24" s="62">
         <v>3</v>
       </c>
-      <c r="C24" s="62" t="s">
+      <c r="C24" s="58" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="7"/>
@@ -2206,7 +2210,7 @@
       <c r="O24" s="36"/>
       <c r="P24" s="36"/>
       <c r="Q24" s="36"/>
-      <c r="R24" s="8"/>
+      <c r="R24" s="36"/>
       <c r="S24" s="11"/>
       <c r="T24" s="11"/>
       <c r="U24" s="28"/>
@@ -2230,9 +2234,9 @@
       <c r="AM24" s="9"/>
     </row>
     <row r="25" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="61"/>
-      <c r="B25" s="56"/>
-      <c r="C25" s="63"/>
+      <c r="A25" s="70"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="59"/>
       <c r="D25" s="12"/>
       <c r="E25" s="29"/>
       <c r="F25" s="23"/>
@@ -2247,17 +2251,17 @@
       <c r="O25" s="37"/>
       <c r="P25" s="37"/>
       <c r="Q25" s="37"/>
-      <c r="R25" s="13"/>
+      <c r="R25" s="37"/>
       <c r="S25" s="13"/>
       <c r="T25" s="13"/>
       <c r="U25" s="29"/>
       <c r="V25" s="23"/>
       <c r="W25" s="13"/>
       <c r="X25" s="13"/>
-      <c r="Y25" s="13"/>
-      <c r="Z25" s="13"/>
-      <c r="AA25" s="13"/>
-      <c r="AB25" s="29"/>
+      <c r="Y25" s="75"/>
+      <c r="Z25" s="49"/>
+      <c r="AA25" s="49"/>
+      <c r="AB25" s="43"/>
       <c r="AC25" s="23"/>
       <c r="AD25" s="13"/>
       <c r="AE25" s="13"/>
@@ -2271,13 +2275,13 @@
       <c r="AM25" s="14"/>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A26" s="68" t="s">
+      <c r="A26" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="57">
+      <c r="B26" s="65">
         <v>1</v>
       </c>
-      <c r="C26" s="65" t="s">
+      <c r="C26" s="63" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="15"/>
@@ -2294,7 +2298,7 @@
       <c r="O26" s="35"/>
       <c r="P26" s="35"/>
       <c r="Q26" s="35"/>
-      <c r="R26" s="5"/>
+      <c r="R26" s="35"/>
       <c r="S26" s="5"/>
       <c r="T26" s="5"/>
       <c r="U26" s="26"/>
@@ -2318,9 +2322,9 @@
       <c r="AM26" s="20"/>
     </row>
     <row r="27" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="69"/>
-      <c r="B27" s="58"/>
-      <c r="C27" s="66"/>
+      <c r="A27" s="72"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="64"/>
       <c r="D27" s="12"/>
       <c r="E27" s="29"/>
       <c r="F27" s="23"/>
@@ -2335,17 +2339,17 @@
       <c r="O27" s="37"/>
       <c r="P27" s="37"/>
       <c r="Q27" s="37"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13"/>
-      <c r="U27" s="29"/>
-      <c r="V27" s="23"/>
-      <c r="W27" s="13"/>
-      <c r="X27" s="13"/>
-      <c r="Y27" s="13"/>
-      <c r="Z27" s="13"/>
-      <c r="AA27" s="13"/>
-      <c r="AB27" s="29"/>
+      <c r="R27" s="37"/>
+      <c r="S27" s="75"/>
+      <c r="T27" s="75"/>
+      <c r="U27" s="76"/>
+      <c r="V27" s="77"/>
+      <c r="W27" s="49"/>
+      <c r="X27" s="49"/>
+      <c r="Y27" s="49"/>
+      <c r="Z27" s="49"/>
+      <c r="AA27" s="49"/>
+      <c r="AB27" s="43"/>
       <c r="AC27" s="23"/>
       <c r="AD27" s="13"/>
       <c r="AE27" s="13"/>
@@ -2359,13 +2363,13 @@
       <c r="AM27" s="14"/>
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A28" s="59" t="s">
+      <c r="A28" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="64">
+      <c r="B28" s="61">
         <v>1</v>
       </c>
-      <c r="C28" s="67" t="s">
+      <c r="C28" s="60" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="17"/>
@@ -2382,7 +2386,7 @@
       <c r="O28" s="38"/>
       <c r="P28" s="38"/>
       <c r="Q28" s="38"/>
-      <c r="R28" s="18"/>
+      <c r="R28" s="38"/>
       <c r="S28" s="18"/>
       <c r="T28" s="18"/>
       <c r="U28" s="31"/>
@@ -2406,52 +2410,52 @@
       <c r="AM28" s="6"/>
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A29" s="60"/>
-      <c r="B29" s="55"/>
-      <c r="C29" s="62"/>
+      <c r="A29" s="69"/>
+      <c r="B29" s="62"/>
+      <c r="C29" s="58"/>
       <c r="D29" s="46"/>
       <c r="E29" s="47"/>
       <c r="F29" s="48"/>
       <c r="G29" s="50"/>
       <c r="H29" s="50"/>
       <c r="I29" s="51"/>
-      <c r="J29" s="74"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="22"/>
+      <c r="J29" s="78"/>
+      <c r="K29" s="50"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="51"/>
+      <c r="N29" s="78"/>
       <c r="O29" s="36"/>
       <c r="P29" s="36"/>
       <c r="Q29" s="36"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="8"/>
-      <c r="U29" s="27"/>
-      <c r="V29" s="22"/>
-      <c r="W29" s="8"/>
-      <c r="X29" s="8"/>
-      <c r="Y29" s="8"/>
-      <c r="Z29" s="8"/>
-      <c r="AA29" s="8"/>
-      <c r="AB29" s="27"/>
+      <c r="R29" s="36"/>
+      <c r="S29" s="50"/>
+      <c r="T29" s="50"/>
+      <c r="U29" s="51"/>
+      <c r="V29" s="78"/>
+      <c r="W29" s="50"/>
+      <c r="X29" s="50"/>
+      <c r="Y29" s="50"/>
+      <c r="Z29" s="50"/>
+      <c r="AA29" s="50"/>
+      <c r="AB29" s="51"/>
       <c r="AC29" s="22"/>
       <c r="AD29" s="8"/>
-      <c r="AE29" s="8"/>
-      <c r="AF29" s="8"/>
-      <c r="AG29" s="8"/>
-      <c r="AH29" s="8"/>
-      <c r="AI29" s="8"/>
-      <c r="AJ29" s="8"/>
-      <c r="AK29" s="8"/>
-      <c r="AL29" s="8"/>
-      <c r="AM29" s="9"/>
+      <c r="AE29" s="54"/>
+      <c r="AF29" s="54"/>
+      <c r="AG29" s="54"/>
+      <c r="AH29" s="54"/>
+      <c r="AI29" s="54"/>
+      <c r="AJ29" s="54"/>
+      <c r="AK29" s="54"/>
+      <c r="AL29" s="54"/>
+      <c r="AM29" s="80"/>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A30" s="60"/>
-      <c r="B30" s="55">
+      <c r="A30" s="69"/>
+      <c r="B30" s="62">
         <v>2</v>
       </c>
-      <c r="C30" s="62" t="s">
+      <c r="C30" s="58" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="7"/>
@@ -2468,7 +2472,7 @@
       <c r="O30" s="36"/>
       <c r="P30" s="36"/>
       <c r="Q30" s="36"/>
-      <c r="R30" s="8"/>
+      <c r="R30" s="36"/>
       <c r="S30" s="8"/>
       <c r="T30" s="8"/>
       <c r="U30" s="27"/>
@@ -2492,9 +2496,9 @@
       <c r="AM30" s="19"/>
     </row>
     <row r="31" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="61"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="63"/>
+      <c r="A31" s="70"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="59"/>
       <c r="D31" s="12"/>
       <c r="E31" s="29"/>
       <c r="F31" s="23"/>
@@ -2509,7 +2513,7 @@
       <c r="O31" s="37"/>
       <c r="P31" s="37"/>
       <c r="Q31" s="37"/>
-      <c r="R31" s="13"/>
+      <c r="R31" s="37"/>
       <c r="S31" s="13"/>
       <c r="T31" s="13"/>
       <c r="U31" s="29"/>
@@ -2580,54 +2584,54 @@
         <v>27</v>
       </c>
       <c r="G36" s="34"/>
-      <c r="J36" s="54" t="s">
+      <c r="J36" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="K36" s="54"/>
-      <c r="L36" s="54"/>
-      <c r="M36" s="54"/>
-      <c r="N36" s="54" t="s">
+      <c r="K36" s="73"/>
+      <c r="L36" s="73"/>
+      <c r="M36" s="73"/>
+      <c r="N36" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="O36" s="54"/>
-      <c r="P36" s="54"/>
-      <c r="Q36" s="54"/>
-      <c r="R36" s="54"/>
-      <c r="V36" s="54" t="s">
+      <c r="O36" s="73"/>
+      <c r="P36" s="73"/>
+      <c r="Q36" s="73"/>
+      <c r="R36" s="73"/>
+      <c r="V36" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="W36" s="54"/>
-      <c r="X36" s="54"/>
-      <c r="Y36" s="54"/>
-      <c r="Z36" s="54"/>
-      <c r="AC36" s="54" t="s">
+      <c r="W36" s="73"/>
+      <c r="X36" s="73"/>
+      <c r="Y36" s="73"/>
+      <c r="Z36" s="73"/>
+      <c r="AC36" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="AD36" s="54"/>
-      <c r="AE36" s="54"/>
-      <c r="AF36" s="54"/>
-      <c r="AG36" s="54"/>
+      <c r="AD36" s="73"/>
+      <c r="AE36" s="73"/>
+      <c r="AF36" s="73"/>
+      <c r="AG36" s="73"/>
     </row>
     <row r="37" spans="5:33" x14ac:dyDescent="0.3">
-      <c r="J37" s="54"/>
-      <c r="K37" s="54"/>
-      <c r="L37" s="54"/>
-      <c r="M37" s="54"/>
-      <c r="N37" s="54"/>
-      <c r="O37" s="54"/>
-      <c r="P37" s="54"/>
-      <c r="Q37" s="54"/>
-      <c r="R37" s="54"/>
-      <c r="V37" s="54"/>
-      <c r="W37" s="54"/>
-      <c r="X37" s="54"/>
-      <c r="Y37" s="54"/>
-      <c r="Z37" s="54"/>
-      <c r="AC37" s="54"/>
-      <c r="AD37" s="54"/>
-      <c r="AE37" s="54"/>
-      <c r="AF37" s="54"/>
-      <c r="AG37" s="54"/>
+      <c r="J37" s="73"/>
+      <c r="K37" s="73"/>
+      <c r="L37" s="73"/>
+      <c r="M37" s="73"/>
+      <c r="N37" s="73"/>
+      <c r="O37" s="73"/>
+      <c r="P37" s="73"/>
+      <c r="Q37" s="73"/>
+      <c r="R37" s="73"/>
+      <c r="V37" s="73"/>
+      <c r="W37" s="73"/>
+      <c r="X37" s="73"/>
+      <c r="Y37" s="73"/>
+      <c r="Z37" s="73"/>
+      <c r="AC37" s="73"/>
+      <c r="AD37" s="73"/>
+      <c r="AE37" s="73"/>
+      <c r="AF37" s="73"/>
+      <c r="AG37" s="73"/>
     </row>
     <row r="42" spans="5:33" x14ac:dyDescent="0.3">
       <c r="F42" s="2"/>
@@ -2655,6 +2659,36 @@
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="AC36:AF37"/>
+    <mergeCell ref="AG36:AG37"/>
+    <mergeCell ref="J36:M37"/>
+    <mergeCell ref="N36:Q37"/>
+    <mergeCell ref="R36:R37"/>
+    <mergeCell ref="V36:Y37"/>
+    <mergeCell ref="Z36:Z37"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="C20:C21"/>
@@ -2671,39 +2705,9 @@
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="AC36:AF37"/>
-    <mergeCell ref="AG36:AG37"/>
-    <mergeCell ref="J36:M37"/>
-    <mergeCell ref="N36:Q37"/>
-    <mergeCell ref="R36:R37"/>
-    <mergeCell ref="V36:Y37"/>
-    <mergeCell ref="Z36:Z37"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="66" scale="62" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>